<commit_message>
finished big data import, tested with recreating database
</commit_message>
<xml_diff>
--- a/Data/Excel/TournamentCategoryPoints.xlsx
+++ b/Data/Excel/TournamentCategoryPoints.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="5055" windowWidth="23040" windowHeight="5115"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="11505" windowHeight="10185"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -64,9 +64,6 @@
     <t>F</t>
   </si>
   <si>
-    <t>ATP-Fs</t>
-  </si>
-  <si>
     <t>R64</t>
   </si>
   <si>
@@ -74,6 +71,9 @@
   </si>
   <si>
     <t>R16</t>
+  </si>
+  <si>
+    <t>ATP-Finals</t>
   </si>
 </sst>
 </file>
@@ -430,8 +430,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D89"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E68" sqref="E68"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="G42" sqref="G42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -533,7 +533,7 @@
         <v>32</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -547,7 +547,7 @@
         <v>32</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D8">
         <v>20</v>
@@ -561,7 +561,7 @@
         <v>32</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D9">
         <v>45</v>
@@ -687,7 +687,7 @@
         <v>48</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D18">
         <v>10</v>
@@ -701,7 +701,7 @@
         <v>48</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D19">
         <v>20</v>
@@ -715,7 +715,7 @@
         <v>48</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D20">
         <v>45</v>
@@ -841,7 +841,7 @@
         <v>32</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D29">
         <v>0</v>
@@ -855,7 +855,7 @@
         <v>32</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D30">
         <v>45</v>
@@ -869,7 +869,7 @@
         <v>32</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D31">
         <v>90</v>
@@ -995,7 +995,7 @@
         <v>48</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D40">
         <v>20</v>
@@ -1009,7 +1009,7 @@
         <v>48</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D41">
         <v>45</v>
@@ -1023,7 +1023,7 @@
         <v>48</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D42">
         <v>90</v>
@@ -1073,7 +1073,7 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B46">
         <v>8</v>
@@ -1087,7 +1087,7 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B47">
         <v>8</v>
@@ -1101,7 +1101,7 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B48">
         <v>8</v>
@@ -1115,7 +1115,7 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B49">
         <v>8</v>
@@ -1129,7 +1129,7 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B50">
         <v>8</v>
@@ -1143,13 +1143,13 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
+        <v>19</v>
+      </c>
+      <c r="B51">
+        <v>8</v>
+      </c>
+      <c r="C51" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="B51">
-        <v>8</v>
-      </c>
-      <c r="C51" s="2" t="s">
-        <v>17</v>
       </c>
       <c r="D51">
         <v>200</v>
@@ -1157,13 +1157,13 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B52">
         <v>8</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D52">
         <v>200</v>
@@ -1171,13 +1171,13 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B53">
         <v>8</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D53">
         <v>200</v>
@@ -1185,7 +1185,7 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B54">
         <v>8</v>
@@ -1199,7 +1199,7 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B55">
         <v>8</v>
@@ -1213,7 +1213,7 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B56">
         <v>8</v>
@@ -1303,7 +1303,7 @@
         <v>128</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D62">
         <v>90</v>
@@ -1317,7 +1317,7 @@
         <v>128</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D63">
         <v>180</v>
@@ -1331,7 +1331,7 @@
         <v>128</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D64">
         <v>360</v>
@@ -1457,7 +1457,7 @@
         <v>56</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D73">
         <v>45</v>
@@ -1471,7 +1471,7 @@
         <v>56</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D74">
         <v>90</v>
@@ -1485,7 +1485,7 @@
         <v>56</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D75">
         <v>180</v>
@@ -1611,7 +1611,7 @@
         <v>96</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D84">
         <v>45</v>
@@ -1625,7 +1625,7 @@
         <v>96</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D85">
         <v>90</v>
@@ -1639,7 +1639,7 @@
         <v>96</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D86">
         <v>180</v>

</xml_diff>

<commit_message>
added exception handling in all import methods for header formatting, refactored ImportSampleData
</commit_message>
<xml_diff>
--- a/Data/Excel/TournamentCategoryPoints.xlsx
+++ b/Data/Excel/TournamentCategoryPoints.xlsx
@@ -16,64 +16,64 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="20">
   <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>PlayersNumber</t>
+  </si>
+  <si>
+    <t>Round Name</t>
+  </si>
+  <si>
+    <t>ATP-250</t>
+  </si>
+  <si>
+    <t>Q</t>
+  </si>
+  <si>
+    <t>ATP-500</t>
+  </si>
+  <si>
+    <t>Grand Slam</t>
+  </si>
+  <si>
+    <t>Masters-1000</t>
+  </si>
+  <si>
+    <t>Q1</t>
+  </si>
+  <si>
+    <t>Q2</t>
+  </si>
+  <si>
+    <t>Q3</t>
+  </si>
+  <si>
+    <t>R128</t>
+  </si>
+  <si>
+    <t>QF</t>
+  </si>
+  <si>
+    <t>SF</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>R64</t>
+  </si>
+  <si>
+    <t>R32</t>
+  </si>
+  <si>
+    <t>R16</t>
+  </si>
+  <si>
+    <t>ATP-Finals</t>
+  </si>
+  <si>
     <t>Points</t>
-  </si>
-  <si>
-    <t>Category</t>
-  </si>
-  <si>
-    <t>PlayersNumber</t>
-  </si>
-  <si>
-    <t>Round Name</t>
-  </si>
-  <si>
-    <t>ATP-250</t>
-  </si>
-  <si>
-    <t>Q</t>
-  </si>
-  <si>
-    <t>ATP-500</t>
-  </si>
-  <si>
-    <t>Grand Slam</t>
-  </si>
-  <si>
-    <t>Masters-1000</t>
-  </si>
-  <si>
-    <t>Q1</t>
-  </si>
-  <si>
-    <t>Q2</t>
-  </si>
-  <si>
-    <t>Q3</t>
-  </si>
-  <si>
-    <t>R128</t>
-  </si>
-  <si>
-    <t>QF</t>
-  </si>
-  <si>
-    <t>SF</t>
-  </si>
-  <si>
-    <t>F</t>
-  </si>
-  <si>
-    <t>R64</t>
-  </si>
-  <si>
-    <t>R32</t>
-  </si>
-  <si>
-    <t>R16</t>
-  </si>
-  <si>
-    <t>ATP-Finals</t>
   </si>
 </sst>
 </file>
@@ -430,8 +430,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="G42" sqref="G42"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -443,27 +443,27 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>3</v>
-      </c>
       <c r="D1" s="1" t="s">
-        <v>0</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B2">
         <v>32</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -471,13 +471,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3">
         <v>32</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -485,13 +485,13 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4">
         <v>32</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D4">
         <v>10</v>
@@ -499,13 +499,13 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>32</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>4</v>
-      </c>
-      <c r="B5">
-        <v>32</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>5</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -513,13 +513,13 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B6">
         <v>32</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -527,13 +527,13 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B7">
         <v>32</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -541,13 +541,13 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B8">
         <v>32</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D8">
         <v>20</v>
@@ -555,13 +555,13 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B9">
         <v>32</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D9">
         <v>45</v>
@@ -569,13 +569,13 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B10">
         <v>32</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D10">
         <v>90</v>
@@ -583,13 +583,13 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B11">
         <v>32</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D11">
         <v>150</v>
@@ -597,13 +597,13 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B12">
         <v>32</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D12">
         <v>250</v>
@@ -611,13 +611,13 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B13">
         <v>48</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D13">
         <v>6</v>
@@ -625,13 +625,13 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B14">
         <v>48</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D14">
         <v>0</v>
@@ -639,13 +639,13 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B15">
         <v>48</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D15">
         <v>20</v>
@@ -653,13 +653,13 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>3</v>
+      </c>
+      <c r="B16">
+        <v>48</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>4</v>
-      </c>
-      <c r="B16">
-        <v>48</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>5</v>
       </c>
       <c r="D16">
         <v>0</v>
@@ -667,13 +667,13 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B17">
         <v>48</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D17">
         <v>0</v>
@@ -681,13 +681,13 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B18">
         <v>48</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D18">
         <v>10</v>
@@ -695,13 +695,13 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B19">
         <v>48</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D19">
         <v>20</v>
@@ -709,13 +709,13 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B20">
         <v>48</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D20">
         <v>45</v>
@@ -723,13 +723,13 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B21">
         <v>48</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D21">
         <v>90</v>
@@ -737,13 +737,13 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B22">
         <v>48</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D22">
         <v>150</v>
@@ -751,13 +751,13 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B23">
         <v>48</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D23">
         <v>250</v>
@@ -765,13 +765,13 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B24">
         <v>32</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D24">
         <v>3</v>
@@ -779,13 +779,13 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B25">
         <v>32</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D25">
         <v>0</v>
@@ -793,13 +793,13 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B26">
         <v>32</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D26">
         <v>10</v>
@@ -807,13 +807,13 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B27">
         <v>32</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D27">
         <v>0</v>
@@ -821,13 +821,13 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B28">
         <v>32</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D28">
         <v>0</v>
@@ -835,13 +835,13 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B29">
         <v>32</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D29">
         <v>0</v>
@@ -849,13 +849,13 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B30">
         <v>32</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D30">
         <v>45</v>
@@ -863,13 +863,13 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B31">
         <v>32</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D31">
         <v>90</v>
@@ -877,13 +877,13 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B32">
         <v>32</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D32">
         <v>180</v>
@@ -891,13 +891,13 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B33">
         <v>32</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D33">
         <v>300</v>
@@ -905,13 +905,13 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B34">
         <v>32</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D34">
         <v>500</v>
@@ -919,13 +919,13 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B35">
         <v>48</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D35">
         <v>10</v>
@@ -933,13 +933,13 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B36">
         <v>48</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D36">
         <v>0</v>
@@ -947,13 +947,13 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B37">
         <v>48</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D37">
         <v>0</v>
@@ -961,13 +961,13 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B38">
         <v>48</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D38">
         <v>0</v>
@@ -975,13 +975,13 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B39">
         <v>48</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D39">
         <v>0</v>
@@ -989,13 +989,13 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B40">
         <v>48</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D40">
         <v>20</v>
@@ -1003,13 +1003,13 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B41">
         <v>48</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D41">
         <v>45</v>
@@ -1017,13 +1017,13 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B42">
         <v>48</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D42">
         <v>90</v>
@@ -1031,13 +1031,13 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B43">
         <v>48</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D43">
         <v>180</v>
@@ -1045,13 +1045,13 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B44">
         <v>48</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D44">
         <v>300</v>
@@ -1059,13 +1059,13 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B45">
         <v>48</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D45">
         <v>500</v>
@@ -1073,13 +1073,13 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B46">
         <v>8</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D46">
         <v>200</v>
@@ -1087,13 +1087,13 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B47">
         <v>8</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D47">
         <v>200</v>
@@ -1101,13 +1101,13 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B48">
         <v>8</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D48">
         <v>200</v>
@@ -1115,13 +1115,13 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B49">
         <v>8</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D49">
         <v>200</v>
@@ -1129,13 +1129,13 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B50">
         <v>8</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D50">
         <v>200</v>
@@ -1143,13 +1143,13 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B51">
         <v>8</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D51">
         <v>200</v>
@@ -1157,13 +1157,13 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B52">
         <v>8</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D52">
         <v>200</v>
@@ -1171,13 +1171,13 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B53">
         <v>8</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D53">
         <v>200</v>
@@ -1185,13 +1185,13 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B54">
         <v>8</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D54">
         <v>600</v>
@@ -1199,13 +1199,13 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B55">
         <v>8</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D55">
         <v>1000</v>
@@ -1213,13 +1213,13 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B56">
         <v>8</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D56">
         <v>1500</v>
@@ -1227,13 +1227,13 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B57">
         <v>128</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D57">
         <v>8</v>
@@ -1241,13 +1241,13 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B58">
         <v>128</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D58">
         <v>16</v>
@@ -1255,13 +1255,13 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B59">
         <v>128</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D59">
         <v>25</v>
@@ -1269,13 +1269,13 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B60">
         <v>128</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D60">
         <v>10</v>
@@ -1283,13 +1283,13 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B61">
         <v>128</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D61">
         <v>45</v>
@@ -1297,13 +1297,13 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B62">
         <v>128</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D62">
         <v>90</v>
@@ -1311,13 +1311,13 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B63">
         <v>128</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D63">
         <v>180</v>
@@ -1325,13 +1325,13 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B64">
         <v>128</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D64">
         <v>360</v>
@@ -1339,13 +1339,13 @@
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B65">
         <v>128</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D65">
         <v>720</v>
@@ -1353,13 +1353,13 @@
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B66">
         <v>128</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D66">
         <v>1200</v>
@@ -1367,13 +1367,13 @@
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B67">
         <v>128</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D67">
         <v>2000</v>
@@ -1381,13 +1381,13 @@
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B68">
         <v>56</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D68">
         <v>4</v>
@@ -1395,13 +1395,13 @@
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B69">
         <v>56</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D69">
         <v>0</v>
@@ -1409,13 +1409,13 @@
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B70">
         <v>56</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D70">
         <v>25</v>
@@ -1423,13 +1423,13 @@
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B71">
         <v>56</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D71">
         <v>0</v>
@@ -1437,13 +1437,13 @@
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B72">
         <v>56</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D72">
         <v>10</v>
@@ -1451,13 +1451,13 @@
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B73">
         <v>56</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D73">
         <v>45</v>
@@ -1465,13 +1465,13 @@
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B74">
         <v>56</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D74">
         <v>90</v>
@@ -1479,13 +1479,13 @@
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B75">
         <v>56</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D75">
         <v>180</v>
@@ -1493,13 +1493,13 @@
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B76">
         <v>56</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D76">
         <v>360</v>
@@ -1507,13 +1507,13 @@
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B77">
         <v>56</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D77">
         <v>600</v>
@@ -1521,13 +1521,13 @@
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B78">
         <v>56</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D78">
         <v>1000</v>
@@ -1535,13 +1535,13 @@
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B79">
         <v>96</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D79">
         <v>16</v>
@@ -1549,13 +1549,13 @@
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B80">
         <v>96</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D80">
         <v>0</v>
@@ -1563,13 +1563,13 @@
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B81">
         <v>96</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D81">
         <v>16</v>
@@ -1577,13 +1577,13 @@
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B82">
         <v>96</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D82">
         <v>10</v>
@@ -1591,13 +1591,13 @@
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B83">
         <v>96</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D83">
         <v>25</v>
@@ -1605,13 +1605,13 @@
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B84">
         <v>96</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D84">
         <v>45</v>
@@ -1619,13 +1619,13 @@
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B85">
         <v>96</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D85">
         <v>90</v>
@@ -1633,13 +1633,13 @@
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B86">
         <v>96</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D86">
         <v>180</v>
@@ -1647,13 +1647,13 @@
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B87">
         <v>96</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D87">
         <v>360</v>
@@ -1661,13 +1661,13 @@
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B88">
         <v>96</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D88">
         <v>600</v>
@@ -1675,13 +1675,13 @@
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B89">
         <v>96</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D89">
         <v>1000</v>

</xml_diff>